<commit_message>
Update ideal budget: replace 1 youth mentor with front desk receptionist
Changes ideal staffing from 4 youth mentors to 3 youth mentors + 1 front
desk receptionist. This provides administrative support and check-in
services while maintaining 6 total staff for ideal programming.

Budget Impact:
- Necessity: $191,528 (unchanged)
- Ideal: $301,854 (decreased from $305,180)
- Savings: $3,326 from lower receptionist wage rate

Staffing Updates:
- Ideal now has 3 youth mentors instead of 4
- Added front desk receptionist at $18/hr (same schedule as mentors)
- All sheets updated: Staffing Costs, Operations Schedule, Expense Detail

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/budget-proposal/op-budget-v5.xlsx
+++ b/budget-proposal/op-budget-v5.xlsx
@@ -1214,18 +1214,18 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>4 mentors for better ratios</t>
+          <t>3 mentors for program support</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="E13" t="inlineStr">
         <is>
-          <t>Teen Coordinator</t>
+          <t>Front Desk Receptionist</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1233,6 +1233,21 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>Administrative support &amp; check-in</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Teen Coordinator</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>Specialized teen programming</t>
         </is>
       </c>
@@ -1356,24 +1371,39 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>4 mentors for activities</t>
+          <t>3 mentors for activities</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="E24" t="inlineStr">
         <is>
-          <t>Teen Coordinator</t>
+          <t>Front Desk Receptionist</t>
         </is>
       </c>
       <c r="F24" t="n">
         <v>1</v>
       </c>
       <c r="H24" t="inlineStr">
+        <is>
+          <t>Administrative support &amp; check-in</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Teen Coordinator</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>Teen-specific activities</t>
         </is>
@@ -2205,7 +2235,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2395,17 +2425,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Additional Youth Mentors (2 positions)</t>
+          <t>Additional Youth Mentor (1 position)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.269</v>
+        <v>0.635</v>
       </c>
       <c r="C6" t="n">
         <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>52800</v>
+        <v>26400</v>
       </c>
       <c r="E6" t="n">
         <v>0.18</v>
@@ -2416,12 +2446,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Program Fees</t>
+          <t>Ideal</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ideal</t>
+          <t>20 hrs/wk (38 wks) + 40 hrs/wk (14 wks) = 1,320 hrs/year</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -2438,17 +2468,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Teen Coordinator</t>
+          <t>Front Desk Receptionist</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.635</v>
       </c>
       <c r="C7" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" t="n">
-        <v>37400</v>
+        <v>23760</v>
       </c>
       <c r="E7" t="n">
         <v>0.18</v>
@@ -2459,55 +2489,92 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Ideal</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>20 hrs/wk (38 wks) + 40 hrs/wk (14 wks) = 1,320 hrs/year</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>30 hrs/wk (38 wks) + 40 hrs/wk (14 wks)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Ideal</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Teen Coordinator</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8169999999999999</v>
+      </c>
+      <c r="C8" t="n">
+        <v>22</v>
+      </c>
+      <c r="D8" t="n">
+        <v>37400</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="F8">
+        <f>D8*(1+E8+Assumptions!$C$8)</f>
+        <v/>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Grants</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Ideal</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>30 hrs/wk (38 wks) + 40 hrs/wk (14 wks)</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Ideal</t>
-        </is>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="6" t="n"/>
+      <c r="F9" s="7" t="n"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>2 Directors + 2 Youth Mentors (required staff)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>NECESSITY BUDGET TOTAL</t>
         </is>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="9">
         <f>F2+F3+F4</f>
         <v/>
       </c>
-      <c r="I9" s="14" t="inlineStr">
-        <is>
-          <t>2 Directors + 2 Youth Mentors (required staff)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="I10" s="15" t="inlineStr">
+        <is>
+          <t>Add 2 more Youth Mentors + Teen Coordinator (full staffing)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>IDEAL BUDGET TOTAL</t>
         </is>
       </c>
-      <c r="F10" s="9">
-        <f>F2+F3+F4+F6+F7</f>
-        <v/>
-      </c>
-      <c r="I10" s="15" t="inlineStr">
-        <is>
-          <t>Add 2 more Youth Mentors + Teen Coordinator (full staffing)</t>
-        </is>
+      <c r="F11">
+        <f>F2+F3+F4+F6+F7+F8</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2880,7 +2947,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Additional Youth Mentors (2)</t>
+          <t>Additional Youth Mentor (1)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2959,7 +3026,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Teen Coordinator</t>
+          <t>Front Desk Receptionist</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3030,6 +3097,75 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Personnel</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Teen Coordinator</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hourly</t>
+        </is>
+      </c>
+      <c r="D8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="E8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="G8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="H8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="I8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="J8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="K8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="L8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="M8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="N8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="O8">
+        <f>'Staffing Costs'!F8/12</f>
+        <v/>
+      </c>
+      <c r="P8">
+        <f>'Staffing Costs'!F8</f>
+        <v/>
+      </c>
+    </row>
     <row r="9">
       <c r="A9" s="18" t="inlineStr">
         <is>
@@ -3457,55 +3593,55 @@
         </is>
       </c>
       <c r="D22">
-        <f>D21+D6+D7</f>
+        <f>D21+D6+D7+D8</f>
         <v/>
       </c>
       <c r="E22">
-        <f>E21+E6+E7</f>
+        <f>E21+E6+E7+E8</f>
         <v/>
       </c>
       <c r="F22">
-        <f>F21+F6+F7</f>
+        <f>F21+F6+F7+F8</f>
         <v/>
       </c>
       <c r="G22">
-        <f>G21+G6+G7</f>
+        <f>G21+G6+G7+G8</f>
         <v/>
       </c>
       <c r="H22">
-        <f>H21+H6+H7</f>
+        <f>H21+H6+H7+H8</f>
         <v/>
       </c>
       <c r="I22">
-        <f>I21+I6+I7</f>
+        <f>I21+I6+I7+I8</f>
         <v/>
       </c>
       <c r="J22">
-        <f>J21+J6+J7</f>
+        <f>J21+J6+J7+J8</f>
         <v/>
       </c>
       <c r="K22">
-        <f>K21+K6+K7</f>
+        <f>K21+K6+K7+K8</f>
         <v/>
       </c>
       <c r="L22">
-        <f>L21+L6+L7</f>
+        <f>L21+L6+L7+L8</f>
         <v/>
       </c>
       <c r="M22">
-        <f>M21+M6+M7</f>
+        <f>M21+M6+M7+M8</f>
         <v/>
       </c>
       <c r="N22">
-        <f>N21+N6+N7</f>
+        <f>N21+N6+N7+N8</f>
         <v/>
       </c>
       <c r="O22">
-        <f>O21+O6+O7</f>
+        <f>O21+O6+O7+O8</f>
         <v/>
       </c>
       <c r="P22" s="9">
-        <f>SUM(D22:O22)</f>
+        <f>P21+P6+P7+P8</f>
         <v/>
       </c>
       <c r="R22" t="inlineStr">

</xml_diff>